<commit_message>
update_A Simple Transformer-style Network for Lightweight Image Super-resolution
</commit_message>
<xml_diff>
--- a/CV/Lightweight/assets/IR_SR_Lightweight_Result.xlsx
+++ b/CV/Lightweight/assets/IR_SR_Lightweight_Result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13160" firstSheet="7" activeTab="8"/>
+    <workbookView windowWidth="27660" windowHeight="13640"/>
   </bookViews>
   <sheets>
     <sheet name="SR" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="68">
   <si>
     <t>Method</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>LatticeNet-CL+</t>
+  </si>
+  <si>
+    <t>STSN</t>
   </si>
   <si>
     <t>Compacter</t>
@@ -1444,10 +1447,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BB13"/>
+  <dimension ref="A1:BB14"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2575,110 +2578,116 @@
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
-        <v>393</v>
-      </c>
-      <c r="D10" s="2"/>
+      <c r="C10" s="1">
+        <v>881.9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>197.7</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
-        <v>38.24</v>
+        <v>38.19</v>
       </c>
       <c r="G10" s="2">
-        <v>0.9619</v>
+        <v>0.9611</v>
       </c>
       <c r="H10" s="2">
-        <v>34.08</v>
+        <v>33.78</v>
       </c>
       <c r="I10" s="2">
-        <v>0.9215</v>
+        <v>0.9199</v>
       </c>
       <c r="J10" s="2">
-        <v>32.35</v>
+        <v>32.3</v>
       </c>
       <c r="K10" s="2">
-        <v>0.9026</v>
+        <v>0.9013</v>
       </c>
       <c r="L10" s="2">
-        <v>32.99</v>
+        <v>32.68</v>
       </c>
       <c r="M10" s="2">
-        <v>0.9354</v>
+        <v>0.9336</v>
       </c>
       <c r="N10" s="2">
-        <v>39.4</v>
+        <v>39.13</v>
       </c>
       <c r="O10" s="2">
-        <v>0.9786</v>
-      </c>
-      <c r="P10" s="2">
-        <v>399</v>
-      </c>
-      <c r="Q10" s="2"/>
+        <v>0.9778</v>
+      </c>
+      <c r="P10" s="1">
+        <v>888.7</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>99.9</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2">
-        <v>34.69</v>
+        <v>34.62</v>
       </c>
       <c r="T10" s="2">
-        <v>0.93</v>
+        <v>0.9292</v>
       </c>
       <c r="U10" s="2">
-        <v>30.65</v>
+        <v>30.54</v>
       </c>
       <c r="V10" s="2">
-        <v>0.8477</v>
+        <v>0.8466</v>
       </c>
       <c r="W10" s="2">
-        <v>29.28</v>
+        <v>29.22</v>
       </c>
       <c r="X10" s="2">
-        <v>0.8117</v>
+        <v>0.809</v>
       </c>
       <c r="Y10" s="2">
-        <v>28.9</v>
+        <v>28.59</v>
       </c>
       <c r="Z10" s="2">
-        <v>0.8659</v>
+        <v>0.8621</v>
       </c>
       <c r="AA10" s="2">
-        <v>34.31</v>
+        <v>34.11</v>
       </c>
       <c r="AB10" s="2">
-        <v>0.9487</v>
+        <v>0.948</v>
       </c>
       <c r="AC10" s="2">
-        <v>408</v>
-      </c>
-      <c r="AD10" s="2"/>
+        <v>898.2</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>50.3</v>
+      </c>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2">
-        <v>32.53</v>
+        <v>32.46</v>
       </c>
       <c r="AG10" s="2">
-        <v>0.8994</v>
+        <v>0.8982</v>
       </c>
       <c r="AH10" s="2">
-        <v>28.88</v>
+        <v>28.76</v>
       </c>
       <c r="AI10" s="2">
-        <v>0.7876</v>
+        <v>0.786</v>
       </c>
       <c r="AJ10" s="2">
-        <v>27.76</v>
+        <v>27.68</v>
       </c>
       <c r="AK10" s="2">
-        <v>0.744</v>
+        <v>0.7405</v>
       </c>
       <c r="AL10" s="2">
-        <v>26.69</v>
+        <v>26.39</v>
       </c>
       <c r="AM10" s="2">
-        <v>0.8025</v>
+        <v>0.7971</v>
       </c>
       <c r="AN10" s="2">
-        <v>31.24</v>
+        <v>30.93</v>
       </c>
       <c r="AO10" s="2">
-        <v>0.9148</v>
+        <v>0.9142</v>
       </c>
       <c r="AP10" s="2"/>
       <c r="AQ10" s="2"/>
@@ -2702,115 +2711,109 @@
         <v>17</v>
       </c>
       <c r="C11" s="2">
-        <v>940</v>
-      </c>
-      <c r="D11" s="2">
-        <v>163.4</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <v>38.16</v>
+        <v>38.24</v>
       </c>
       <c r="G11" s="2">
-        <v>0.9612</v>
+        <v>0.9619</v>
       </c>
       <c r="H11" s="2">
-        <v>34</v>
+        <v>34.08</v>
       </c>
       <c r="I11" s="2">
-        <v>0.9213</v>
+        <v>0.9215</v>
       </c>
       <c r="J11" s="2">
-        <v>32.33</v>
+        <v>32.35</v>
       </c>
       <c r="K11" s="2">
-        <v>0.9015</v>
+        <v>0.9026</v>
       </c>
       <c r="L11" s="2">
-        <v>32.81</v>
+        <v>32.99</v>
       </c>
       <c r="M11" s="2">
-        <v>0.9346</v>
+        <v>0.9354</v>
       </c>
       <c r="N11" s="2">
-        <v>39.32</v>
+        <v>39.4</v>
       </c>
       <c r="O11" s="2">
-        <v>0.9783</v>
+        <v>0.9786</v>
       </c>
       <c r="P11" s="2">
-        <v>949</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>77.3</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2">
-        <v>34.63</v>
+        <v>34.69</v>
       </c>
       <c r="T11" s="2">
-        <v>0.929</v>
+        <v>0.93</v>
       </c>
       <c r="U11" s="2">
-        <v>30.6</v>
+        <v>30.65</v>
       </c>
       <c r="V11" s="2">
-        <v>0.8467</v>
+        <v>0.8477</v>
       </c>
       <c r="W11" s="2">
-        <v>29.25</v>
+        <v>29.28</v>
       </c>
       <c r="X11" s="2">
-        <v>0.8093</v>
+        <v>0.8117</v>
       </c>
       <c r="Y11" s="2">
-        <v>28.76</v>
+        <v>28.9</v>
       </c>
       <c r="Z11" s="2">
-        <v>0.8646</v>
+        <v>0.8659</v>
       </c>
       <c r="AA11" s="2">
-        <v>34.3</v>
+        <v>34.31</v>
       </c>
       <c r="AB11" s="2">
-        <v>0.949</v>
+        <v>0.9487</v>
       </c>
       <c r="AC11" s="2">
-        <v>961</v>
-      </c>
-      <c r="AD11" s="2">
-        <v>42.1</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2">
-        <v>32.56</v>
+        <v>32.53</v>
       </c>
       <c r="AG11" s="2">
-        <v>0.8992</v>
+        <v>0.8994</v>
       </c>
       <c r="AH11" s="2">
-        <v>28.83</v>
+        <v>28.88</v>
       </c>
       <c r="AI11" s="2">
-        <v>0.7873</v>
+        <v>0.7876</v>
       </c>
       <c r="AJ11" s="2">
-        <v>27.71</v>
+        <v>27.76</v>
       </c>
       <c r="AK11" s="2">
-        <v>0.7418</v>
+        <v>0.744</v>
       </c>
       <c r="AL11" s="2">
-        <v>26.6</v>
+        <v>26.69</v>
       </c>
       <c r="AM11" s="2">
-        <v>0.8017</v>
+        <v>0.8025</v>
       </c>
       <c r="AN11" s="2">
-        <v>31.17</v>
+        <v>31.24</v>
       </c>
       <c r="AO11" s="2">
-        <v>0.917</v>
+        <v>0.9148</v>
       </c>
       <c r="AP11" s="2"/>
       <c r="AQ11" s="2"/>
@@ -2834,100 +2837,116 @@
         <v>17</v>
       </c>
       <c r="C12" s="2">
-        <v>298</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>940</v>
+      </c>
+      <c r="D12" s="2">
+        <v>163.4</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <v>38.17</v>
+        <v>38.16</v>
       </c>
       <c r="G12" s="2">
-        <v>0.9613</v>
+        <v>0.9612</v>
       </c>
       <c r="H12" s="2">
-        <v>33.96</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2">
-        <v>0.9216</v>
+        <v>0.9213</v>
       </c>
       <c r="J12" s="2">
-        <v>32.31</v>
+        <v>32.33</v>
       </c>
       <c r="K12" s="2">
-        <v>0.9017</v>
+        <v>0.9015</v>
       </c>
       <c r="L12" s="2">
-        <v>32.88</v>
+        <v>32.81</v>
       </c>
       <c r="M12" s="2">
-        <v>0.9353</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+        <v>0.9346</v>
+      </c>
+      <c r="N12" s="2">
+        <v>39.32</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.9783</v>
+      </c>
       <c r="P12" s="2">
-        <v>304</v>
-      </c>
-      <c r="Q12" s="2"/>
+        <v>949</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>77.3</v>
+      </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2">
-        <v>34.58</v>
+        <v>34.63</v>
       </c>
       <c r="T12" s="2">
         <v>0.929</v>
       </c>
       <c r="U12" s="2">
-        <v>30.53</v>
+        <v>30.6</v>
       </c>
       <c r="V12" s="2">
-        <v>0.8465</v>
+        <v>0.8467</v>
       </c>
       <c r="W12" s="2">
-        <v>29.23</v>
+        <v>29.25</v>
       </c>
       <c r="X12" s="2">
-        <v>0.8096</v>
+        <v>0.8093</v>
       </c>
       <c r="Y12" s="2">
-        <v>28.68</v>
+        <v>28.76</v>
       </c>
       <c r="Z12" s="2">
-        <v>0.8633</v>
-      </c>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
+        <v>0.8646</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>34.3</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0.949</v>
+      </c>
       <c r="AC12" s="2">
-        <v>313</v>
-      </c>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2">
-        <v>17.2</v>
-      </c>
+        <v>961</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>42.1</v>
+      </c>
+      <c r="AE12" s="2"/>
       <c r="AF12" s="2">
-        <v>32.39</v>
+        <v>32.56</v>
       </c>
       <c r="AG12" s="2">
-        <v>0.8964</v>
+        <v>0.8992</v>
       </c>
       <c r="AH12" s="2">
-        <v>28.8</v>
+        <v>28.83</v>
       </c>
       <c r="AI12" s="2">
-        <v>0.7865</v>
+        <v>0.7873</v>
       </c>
       <c r="AJ12" s="2">
-        <v>27.7</v>
+        <v>27.71</v>
       </c>
       <c r="AK12" s="2">
         <v>0.7418</v>
       </c>
       <c r="AL12" s="2">
-        <v>26.48</v>
+        <v>26.6</v>
       </c>
       <c r="AM12" s="2">
-        <v>0.7978</v>
-      </c>
-      <c r="AN12" s="2"/>
-      <c r="AO12" s="2"/>
+        <v>0.8017</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>31.17</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>0.917</v>
+      </c>
       <c r="AP12" s="2"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
@@ -2950,97 +2969,97 @@
         <v>17</v>
       </c>
       <c r="C13" s="2">
-        <v>732</v>
+        <v>298</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <v>38.32</v>
+        <v>38.17</v>
       </c>
       <c r="G13" s="2">
-        <v>0.9618</v>
+        <v>0.9613</v>
       </c>
       <c r="H13" s="2">
-        <v>34.24</v>
+        <v>33.96</v>
       </c>
       <c r="I13" s="2">
-        <v>0.9232</v>
+        <v>0.9216</v>
       </c>
       <c r="J13" s="2">
-        <v>32.4</v>
+        <v>32.31</v>
       </c>
       <c r="K13" s="2">
-        <v>0.9028</v>
+        <v>0.9017</v>
       </c>
       <c r="L13" s="2">
-        <v>33.35</v>
+        <v>32.88</v>
       </c>
       <c r="M13" s="2">
-        <v>0.9387</v>
+        <v>0.9353</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2">
-        <v>739</v>
+        <v>304</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2">
-        <v>34.84</v>
+        <v>34.58</v>
       </c>
       <c r="T13" s="2">
-        <v>0.9307</v>
+        <v>0.929</v>
       </c>
       <c r="U13" s="2">
-        <v>30.66</v>
+        <v>30.53</v>
       </c>
       <c r="V13" s="2">
-        <v>0.8491</v>
+        <v>0.8465</v>
       </c>
       <c r="W13" s="2">
-        <v>29.32</v>
+        <v>29.23</v>
       </c>
       <c r="X13" s="2">
-        <v>0.8119</v>
+        <v>0.8096</v>
       </c>
       <c r="Y13" s="2">
-        <v>29.08</v>
+        <v>28.68</v>
       </c>
       <c r="Z13" s="2">
-        <v>0.8706</v>
+        <v>0.8633</v>
       </c>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2">
-        <v>748</v>
+        <v>313</v>
       </c>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2">
-        <v>40.7</v>
+        <v>17.2</v>
       </c>
       <c r="AF13" s="2">
-        <v>32.57</v>
+        <v>32.39</v>
       </c>
       <c r="AG13" s="2">
-        <v>0.899</v>
+        <v>0.8964</v>
       </c>
       <c r="AH13" s="2">
-        <v>28.89</v>
+        <v>28.8</v>
       </c>
       <c r="AI13" s="2">
-        <v>0.7898</v>
+        <v>0.7865</v>
       </c>
       <c r="AJ13" s="2">
-        <v>27.78</v>
+        <v>27.7</v>
       </c>
       <c r="AK13" s="2">
-        <v>0.7449</v>
+        <v>0.7418</v>
       </c>
       <c r="AL13" s="2">
-        <v>26.89</v>
+        <v>26.48</v>
       </c>
       <c r="AM13" s="2">
-        <v>0.8096</v>
+        <v>0.7978</v>
       </c>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
@@ -3057,6 +3076,122 @@
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
       <c r="BB13" s="2"/>
+    </row>
+    <row r="14" spans="1:54">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2">
+        <v>732</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>38.32</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.9618</v>
+      </c>
+      <c r="H14" s="2">
+        <v>34.24</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.9232</v>
+      </c>
+      <c r="J14" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.9028</v>
+      </c>
+      <c r="L14" s="2">
+        <v>33.35</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.9387</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2">
+        <v>739</v>
+      </c>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2">
+        <v>34.84</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.9307</v>
+      </c>
+      <c r="U14" s="2">
+        <v>30.66</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0.8491</v>
+      </c>
+      <c r="W14" s="2">
+        <v>29.32</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0.8119</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>29.08</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0.8706</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2">
+        <v>748</v>
+      </c>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2">
+        <v>40.7</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>32.57</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>0.899</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>28.89</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>0.7898</v>
+      </c>
+      <c r="AJ14" s="2">
+        <v>27.78</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>0.7449</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>26.89</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>0.8096</v>
+      </c>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -3124,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3156,13 +3291,13 @@
     <row r="2" spans="1:28">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3230,11 +3365,11 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
@@ -3242,11 +3377,11 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
@@ -3254,11 +3389,11 @@
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
@@ -3334,10 +3469,10 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3">
         <v>932</v>
@@ -3719,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3732,13 +3867,13 @@
     <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3788,10 +3923,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2">
         <v>370</v>
@@ -3817,10 +3952,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>830</v>
@@ -3846,10 +3981,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2">
         <v>370</v>
@@ -3875,10 +4010,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2">
         <v>830</v>
@@ -3941,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3950,7 +4085,7 @@
     <row r="2" spans="1:5">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -3964,10 +4099,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2">
         <v>830</v>
@@ -3981,10 +4116,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C4" s="2">
         <v>830</v>
@@ -4028,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4038,13 +4173,13 @@
     <row r="2" spans="1:6">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -4055,10 +4190,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="11">
         <v>1934</v>
@@ -4075,10 +4210,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="11">
         <v>3327</v>
@@ -4095,10 +4230,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -4111,10 +4246,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -4157,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4169,20 +4304,20 @@
     <row r="2" spans="1:8">
       <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -4206,10 +4341,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="11">
         <v>912</v>
@@ -4285,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4316,13 +4451,13 @@
     <row r="2" spans="1:27">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -4388,15 +4523,15 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
@@ -4404,15 +4539,15 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
@@ -4420,15 +4555,15 @@
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U4" s="3"/>
       <c r="V4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3" t="s">
@@ -4515,10 +4650,10 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3">
         <v>407</v>
@@ -4598,10 +4733,10 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3">
         <v>935</v>
@@ -4730,7 +4865,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4742,20 +4877,20 @@
     <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -4779,10 +4914,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2">
         <v>407</v>
@@ -4803,10 +4938,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2">
         <v>935</v>
@@ -4863,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4875,20 +5010,20 @@
     <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -4912,10 +5047,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2">
         <v>407</v>
@@ -4936,10 +5071,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2">
         <v>935</v>
@@ -4978,7 +5113,7 @@
   <sheetPr/>
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
@@ -4994,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -5025,13 +5160,13 @@
     <row r="2" spans="1:27">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -5097,15 +5232,15 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
@@ -5113,15 +5248,15 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
@@ -5129,15 +5264,15 @@
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U4" s="3"/>
       <c r="V4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3" t="s">
@@ -5224,13 +5359,13 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>34.23</v>

</xml_diff>